<commit_message>
Test data sheet and locators added/updated
</commit_message>
<xml_diff>
--- a/Instantopen/src/main/java/com/Resources/TestData.xlsx
+++ b/Instantopen/src/main/java/com/Resources/TestData.xlsx
@@ -1350,7 +1350,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1361,7 +1361,7 @@
   <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3236,13 +3236,14 @@
   <dimension ref="A1:AM21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3364,7 +3365,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>111</v>
       </c>
@@ -3447,7 +3448,7 @@
         <v>169</v>
       </c>
       <c r="AE2" s="6" t="s">
-        <v>170</v>
+        <v>193</v>
       </c>
       <c r="AF2" s="6" t="s">
         <v>171</v>
@@ -3465,7 +3466,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>175</v>
       </c>
@@ -3494,7 +3495,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>181</v>
       </c>
@@ -3577,7 +3578,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>201</v>
       </c>
@@ -3609,7 +3610,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>205</v>
       </c>
@@ -3671,7 +3672,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>210</v>
       </c>
@@ -3721,7 +3722,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>223</v>
       </c>
@@ -3738,7 +3739,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="9" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>235</v>
       </c>
@@ -3797,7 +3798,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>236</v>
       </c>
@@ -3823,7 +3824,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="11" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>237</v>
       </c>
@@ -3852,7 +3853,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="12" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>244</v>
       </c>
@@ -3881,7 +3882,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="13" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>252</v>
       </c>
@@ -3937,7 +3938,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="14" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>259</v>
       </c>
@@ -4005,7 +4006,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="15" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>266</v>
       </c>
@@ -4046,7 +4047,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="16" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>276</v>
       </c>
@@ -4090,7 +4091,7 @@
       <c r="AG16" s="9"/>
       <c r="AH16" s="9"/>
     </row>
-    <row r="17" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>282</v>
       </c>
@@ -4137,7 +4138,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="18" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>298</v>
       </c>
@@ -4193,7 +4194,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="19" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>299</v>
       </c>
@@ -4264,7 +4265,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="20" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>307</v>
       </c>
@@ -4305,7 +4306,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="21" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>312</v>
       </c>

</xml_diff>

<commit_message>
New Scripts of Funding Account.
</commit_message>
<xml_diff>
--- a/Instantopen/src/main/java/com/Resources/TestData.xlsx
+++ b/Instantopen/src/main/java/com/Resources/TestData.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2529" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2621" uniqueCount="539">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1630,6 +1630,18 @@
   </si>
   <si>
     <t>C23865_VerifySaveContinueOnSaveProgressPage</t>
+  </si>
+  <si>
+    <t>C23906_VerifyFundTransferWithElectronicCheck</t>
+  </si>
+  <si>
+    <t>C23907_VerifyFundTransferWithDebitCard</t>
+  </si>
+  <si>
+    <t>C23908_VerifyFundTransferOptions</t>
+  </si>
+  <si>
+    <t>C23909_VerifyApplicationSubmittion</t>
   </si>
 </sst>
 </file>
@@ -2013,7 +2025,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2021,10 +2033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F129"/>
+  <dimension ref="A1:F133"/>
   <sheetViews>
-    <sheetView topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127:XFD129"/>
+    <sheetView topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3993,6 +4005,62 @@
         <v>7</v>
       </c>
       <c r="F129" s="1"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>535</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C130" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D130" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>536</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C131" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D131" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>537</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D132" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>538</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D133" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4123,19 +4191,23 @@
     <hyperlink ref="B127" r:id="rId125"/>
     <hyperlink ref="B128" r:id="rId126"/>
     <hyperlink ref="B129" r:id="rId127"/>
+    <hyperlink ref="B130" r:id="rId128"/>
+    <hyperlink ref="B131" r:id="rId129"/>
+    <hyperlink ref="B132" r:id="rId130"/>
+    <hyperlink ref="B133" r:id="rId131"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId128"/>
+  <pageSetup orientation="portrait" r:id="rId132"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD97"/>
+  <dimension ref="A1:AD101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A95" sqref="A95:XFD97"/>
+      <selection pane="bottomLeft" activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8884,6 +8956,242 @@
         <v>82</v>
       </c>
     </row>
+    <row r="98" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="I98" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="J98" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K98" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L98" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M98" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N98" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O98" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P98" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q98" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R98" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S98" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T98" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X98" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y98" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z98" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="99" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="I99" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="J99" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K99" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L99" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M99" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N99" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O99" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P99" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q99" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R99" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S99" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T99" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X99" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y99" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z99" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="100" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="I100" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="J100" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K100" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L100" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M100" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N100" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O100" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P100" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q100" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R100" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S100" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T100" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X100" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y100" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z100" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="101" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
+        <v>538</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="J101" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K101" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L101" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M101" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N101" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O101" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P101" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q101" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R101" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S101" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T101" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X101" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y101" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z101" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8973,7 +9281,7 @@
   <dimension ref="A1:AM21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10081,7 +10389,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="W11" sqref="W11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>